<commit_message>
BOM - Co mame
</commit_message>
<xml_diff>
--- a/- DOCS -/component_list/to_buy_other.xlsx
+++ b/- DOCS -/component_list/to_buy_other.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Simak\OneDrive\Dokumenty\GitHub\RoboCop\- DOCS -\components\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MenMe\Рабочий стол\GitHub\RoboCop\- DOCS -\component_list\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F891449-E29C-4CC5-A7AD-23478E8F81BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81DE8085-812A-47B3-861C-C705B2BDE00D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{29776EEE-8C0F-469C-B67E-A0A36D074C22}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{29776EEE-8C0F-469C-B67E-A0A36D074C22}"/>
   </bookViews>
   <sheets>
     <sheet name="List1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>name</t>
   </si>
@@ -48,6 +48,15 @@
   </si>
   <si>
     <t>note</t>
+  </si>
+  <si>
+    <t>xt30 f</t>
+  </si>
+  <si>
+    <t>xt30 m</t>
+  </si>
+  <si>
+    <t>Conn_01x06_Pin</t>
   </si>
 </sst>
 </file>
@@ -512,27 +521,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B94A6B9C-3679-4967-B1B1-EEFA0AB8BF45}">
-  <dimension ref="B1:E3"/>
+  <dimension ref="B1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="27.21875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="27.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="4.21875" customWidth="1"/>
-    <col min="2" max="2" width="27.21875" style="5"/>
-    <col min="3" max="4" width="27.21875" style="6"/>
-    <col min="5" max="5" width="27.21875" style="7"/>
+    <col min="1" max="1" width="4.1796875" customWidth="1"/>
+    <col min="2" max="2" width="27.1796875" style="5"/>
+    <col min="3" max="4" width="27.1796875" style="6"/>
+    <col min="5" max="5" width="27.1796875" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B1"/>
       <c r="C1"/>
       <c r="D1"/>
       <c r="E1"/>
     </row>
-    <row r="2" spans="2:5" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:5" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -546,11 +555,31 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="2:5" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="2"/>
-      <c r="C3" s="3"/>
+    <row r="3" spans="2:5" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="B3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="3">
+        <v>5</v>
+      </c>
       <c r="D3" s="3"/>
       <c r="E3" s="4"/>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B4" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B5" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="6">
+        <v>15</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>